<commit_message>
The test plan added
</commit_message>
<xml_diff>
--- a/Testing_of_TimeOff.Management.xlsx
+++ b/Testing_of_TimeOff.Management.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18720" windowHeight="7245"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="18720" windowHeight="7245" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test cases" sheetId="1" r:id="rId1"/>
@@ -6392,7 +6392,7 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
@@ -10135,9 +10135,9 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>